<commit_message>
add try-except without alphanumeric ID
</commit_message>
<xml_diff>
--- a/data/message-text.xlsx
+++ b/data/message-text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JMargutti\OneDrive - Rode Kruis\Rode Kruis\NS-support\HSP@Sea\ocean-viking-messaging\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C23469-3CAB-4829-A83A-31F6AFC94154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE20DF2-ECAF-4246-84CD-DBAFA46DF7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{70D7A4BB-17E5-4BF2-8E26-4D150AF0FA58}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{70D7A4BB-17E5-4BF2-8E26-4D150AF0FA58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>somali</t>
   </si>
   <si>
-    <t>Hello, this is a message from the Red Cross Red Crescent. 123 has been rescued by the rescue ship "Ocean Viking" in the Mediterranean sea and is alive and well. 123 will contact you whenever possible. Please do not reply to this message, you will not receive an answer.</t>
-  </si>
-  <si>
     <t>tigrinya</t>
   </si>
   <si>
@@ -75,16 +72,22 @@
     <t>farsi</t>
   </si>
   <si>
-    <t>Bonjour, ceci est un message de la Croix-Rouge et du Croissant-Rouge. 123 a été secouru par le navire de sauvetage "Ocean Viking" dans la mer Méditerranée et est sain et sauf. 123 vous contactera dès que possible. Merci de ne pas répondre à ce message, vous ne recevrez pas de réponse.</t>
-  </si>
-  <si>
     <t>from</t>
   </si>
   <si>
     <t>OceanViking</t>
   </si>
   <si>
-    <t>مرحبًا ، هذه رسالة من الصليب الأحمر والهلال الأحمر. أنقذت سفينة الإنقاذ "أوشن فايكنغ" 123 في البحر الأبيض المتوسط وهو/هي على قيد الحياة وبصحة جيدة. 123 سيتصل/ستتصل بكم عندما يمكن فعل ذلك. الرجاء عدم الرد على هذه الرسالة، فلن تتلقى إجابة.</t>
+    <t>Hello, this is a message from the International Federation of the Red Cross and Red Crescent. 123 has been rescued by the rescue ship "Ocean Viking" in the Mediterranean sea and is alive and well. 123 will contact you whenever possible. Please do not reply to this message, you will not receive an answer.</t>
+  </si>
+  <si>
+    <t>Bonjour, ceci est un message de la Federation Internationale de la Croix-Rouge et du Croissant-Rouge. 123 a été secouru par le navire de sauvetage "Ocean Viking" dans la mer Méditerranée et est sain et sauf. 123 vous contactera dès que possible. Merci de ne pas répondre à ce message, vous ne recevrez pas de réponse.</t>
+  </si>
+  <si>
+    <t>مرحبًا ، هذه رسالة من الاتحاد الدولي للصليب الأحمر والهلال الأحمر.
+لقد أنقذت سفينة الإنقاذ "أوشن فايكنغ" 123 في البحر الأبيض المتوسط وهو/هي على قيد الحياة وبصحة جيدة. 
+123 سيتصل/ستتصل بكم عندما يمكن فعل ذلك. 
+الرجاء عدم الرد على هذه الرسالة، فلن تتلقى إجابة.</t>
   </si>
 </sst>
 </file>
@@ -120,8 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,61 +445,61 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="168.20703125" customWidth="1"/>
+    <col min="2" max="2" width="69.734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -508,22 +514,22 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>